<commit_message>
AutoCommit_3 июля 2023 г. 16:22:29_SibNout2020
</commit_message>
<xml_diff>
--- a/3ПКС-120/УП_/3ПКС-120_Уп.xlsx
+++ b/3ПКС-120/УП_/3ПКС-120_Уп.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Git_Hub_V2\KipFin_Lab_2023_v0_Git0\3ПКС-120\УП_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A7ABAEA-A565-498A-9577-DB83ABD3D338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E3A404-66AA-47A7-BCEE-874C65910D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -487,7 +487,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E24" sqref="E24"/>
+      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -558,8 +558,12 @@
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="4">
+        <v>5</v>
+      </c>
+      <c r="D8" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="9" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -578,8 +582,12 @@
       <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
+      <c r="C10" s="4">
+        <v>5</v>
+      </c>
+      <c r="D10" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="11" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
@@ -588,8 +596,12 @@
       <c r="B11" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+      <c r="C11" s="4">
+        <v>5</v>
+      </c>
+      <c r="D11" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="12" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
@@ -598,8 +610,12 @@
       <c r="B12" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="4"/>
+      <c r="C12" s="4">
+        <v>5</v>
+      </c>
+      <c r="D12" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
@@ -608,8 +624,12 @@
       <c r="B13" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
+      <c r="C13" s="4">
+        <v>5</v>
+      </c>
+      <c r="D13" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="14" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
@@ -618,8 +638,12 @@
       <c r="B14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="4"/>
+      <c r="C14" s="4">
+        <v>5</v>
+      </c>
+      <c r="D14" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
@@ -628,8 +652,12 @@
       <c r="B15" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
+      <c r="C15" s="4">
+        <v>5</v>
+      </c>
+      <c r="D15" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="16" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
@@ -638,8 +666,12 @@
       <c r="B16" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="4"/>
+      <c r="C16" s="4">
+        <v>5</v>
+      </c>
+      <c r="D16" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
@@ -648,8 +680,12 @@
       <c r="B17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+      <c r="C17" s="4">
+        <v>5</v>
+      </c>
+      <c r="D17" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
@@ -668,8 +704,12 @@
       <c r="B19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
+      <c r="C19" s="4">
+        <v>5</v>
+      </c>
+      <c r="D19" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
@@ -678,8 +718,12 @@
       <c r="B20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="4"/>
+      <c r="C20" s="4">
+        <v>5</v>
+      </c>
+      <c r="D20" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="21" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
@@ -698,8 +742,12 @@
       <c r="B22" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
+      <c r="C22" s="4">
+        <v>5</v>
+      </c>
+      <c r="D22" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="23" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">

</xml_diff>

<commit_message>
AutoCommit_3 июля 2023 г. 16:31:20_SibNout2020
</commit_message>
<xml_diff>
--- a/3ПКС-120/УП_/3ПКС-120_Уп.xlsx
+++ b/3ПКС-120/УП_/3ПКС-120_Уп.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Git_Hub_V2\KipFin_Lab_2023_v0_Git0\3ПКС-120\УП_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84E3A404-66AA-47A7-BCEE-874C65910D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946D7BEA-A213-40AB-A3DB-D2473A4729D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -487,7 +487,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C8" sqref="C8"/>
+      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -518,8 +518,12 @@
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="C4" s="4">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -528,8 +532,12 @@
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="4">
+        <v>5</v>
+      </c>
+      <c r="D5" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -538,8 +546,12 @@
       <c r="B6" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="C6" s="4">
+        <v>5</v>
+      </c>
+      <c r="D6" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="7" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -548,8 +560,12 @@
       <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="C7" s="4">
+        <v>5</v>
+      </c>
+      <c r="D7" s="4">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -694,7 +710,9 @@
       <c r="B18" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="4"/>
+      <c r="C18" s="4">
+        <v>5</v>
+      </c>
       <c r="D18" s="4"/>
     </row>
     <row r="19" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
AutoCommit_3 июля 2023 г. 16:57:20_SibNout2020
</commit_message>
<xml_diff>
--- a/3ПКС-120/УП_/3ПКС-120_Уп.xlsx
+++ b/3ПКС-120/УП_/3ПКС-120_Уп.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Git_Hub_V2\KipFin_Lab_2023_v0_Git0\3ПКС-120\УП_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946D7BEA-A213-40AB-A3DB-D2473A4729D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B5115F-278A-4884-BA46-DC6A708D2640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Абакумов Кирилл</t>
   </si>
@@ -105,6 +105,12 @@
   </si>
   <si>
     <t>ПП</t>
+  </si>
+  <si>
+    <t>отчислен</t>
+  </si>
+  <si>
+    <t>Сдали комплект</t>
   </si>
 </sst>
 </file>
@@ -481,13 +487,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:D26"/>
+  <dimension ref="A2:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C21" sqref="C21"/>
+      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -499,19 +505,22 @@
     <col min="18" max="19" width="5.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:4" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -524,8 +533,11 @@
       <c r="D4" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -538,8 +550,11 @@
       <c r="D5" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -552,8 +567,11 @@
       <c r="D6" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -566,8 +584,11 @@
       <c r="D7" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -580,18 +601,25 @@
       <c r="D8" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C9" s="4">
+        <v>5</v>
+      </c>
+      <c r="D9" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -604,8 +632,11 @@
       <c r="D10" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -618,8 +649,11 @@
       <c r="D11" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -632,8 +666,11 @@
       <c r="D12" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -646,8 +683,11 @@
       <c r="D13" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E13">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -660,8 +700,11 @@
       <c r="D14" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E14">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -674,8 +717,11 @@
       <c r="D15" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -688,8 +734,11 @@
       <c r="D16" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E16">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -702,8 +751,11 @@
       <c r="D17" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -713,9 +765,11 @@
       <c r="C18" s="4">
         <v>5</v>
       </c>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D18" s="4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -728,8 +782,11 @@
       <c r="D19" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -742,18 +799,23 @@
       <c r="D20" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E20">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>18</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -766,18 +828,23 @@
       <c r="D22" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>20</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4">
+        <v>5</v>
+      </c>
       <c r="D23" s="4"/>
     </row>
-    <row r="24" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -790,8 +857,11 @@
       <c r="D24" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E24">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -804,8 +874,11 @@
       <c r="D25" s="4">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="E25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
AutoCommit_4 июля 2023 г. 9:03:29_SibNout2020
</commit_message>
<xml_diff>
--- a/3ПКС-120/УП_/3ПКС-120_Уп.xlsx
+++ b/3ПКС-120/УП_/3ПКС-120_Уп.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Git_Hub_V2\KipFin_Lab_2023_v0_Git0\3ПКС-120\УП_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59B5115F-278A-4884-BA46-DC6A708D2640}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A0B1A92-BB60-4373-824D-E6608DC52423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -493,7 +493,7 @@
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E16" sqref="E16"/>
+      <selection pane="bottomRight" activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -618,6 +618,9 @@
       <c r="D9" s="4">
         <v>5</v>
       </c>
+      <c r="E9">
+        <v>5</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -768,6 +771,9 @@
       <c r="D18" s="4">
         <v>5</v>
       </c>
+      <c r="E18">
+        <v>5</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
@@ -842,7 +848,12 @@
       <c r="C23" s="4">
         <v>5</v>
       </c>
-      <c r="D23" s="4"/>
+      <c r="D23" s="4">
+        <v>5</v>
+      </c>
+      <c r="E23">
+        <v>5</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">

</xml_diff>

<commit_message>
AutoCommit_5 июля 2023 г. 11:52:36_SibNout2020
</commit_message>
<xml_diff>
--- a/3ПКС-120/УП_/3ПКС-120_Уп.xlsx
+++ b/3ПКС-120/УП_/3ПКС-120_Уп.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\D\Git_Hub_V2\KipFin_Lab_2023_v0_Git0\3ПКС-120\УП_\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B76A62FE-7FF1-4983-9730-1A3B8A436FE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF80BBA1-39D7-4F25-95C1-6BAED75A88A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Абакумов Кирилл</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Сдали комплект</t>
+  </si>
+  <si>
+    <t>Экзамен</t>
   </si>
 </sst>
 </file>
@@ -487,13 +490,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:E26"/>
+  <dimension ref="A2:J26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="2" ySplit="3" topLeftCell="C4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="O8" sqref="O8"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -505,7 +508,7 @@
     <col min="18" max="19" width="5.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" ht="29" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="2" t="s">
         <v>22</v>
       </c>
@@ -515,12 +518,15 @@
       <c r="E2" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="4" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>1</v>
       </c>
@@ -536,8 +542,11 @@
       <c r="E4">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I4">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -553,8 +562,11 @@
       <c r="E5">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -570,8 +582,11 @@
       <c r="E6">
         <v>5</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -587,8 +602,11 @@
       <c r="E7">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -604,8 +622,11 @@
       <c r="E8">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>6</v>
       </c>
@@ -621,8 +642,11 @@
       <c r="E9">
         <v>5</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>7</v>
       </c>
@@ -638,8 +662,11 @@
       <c r="E10">
         <v>5</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>8</v>
       </c>
@@ -655,8 +682,11 @@
       <c r="E11">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>9</v>
       </c>
@@ -672,8 +702,11 @@
       <c r="E12">
         <v>5</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I12">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>10</v>
       </c>
@@ -689,8 +722,11 @@
       <c r="E13">
         <v>5</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I13">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>11</v>
       </c>
@@ -706,8 +742,11 @@
       <c r="E14">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I14">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>12</v>
       </c>
@@ -723,8 +762,11 @@
       <c r="E15">
         <v>5</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I15">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>13</v>
       </c>
@@ -740,8 +782,11 @@
       <c r="E16">
         <v>5</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I16">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>14</v>
       </c>
@@ -757,8 +802,11 @@
       <c r="E17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>15</v>
       </c>
@@ -774,8 +822,11 @@
       <c r="E18">
         <v>5</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>16</v>
       </c>
@@ -791,8 +842,11 @@
       <c r="E19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>17</v>
       </c>
@@ -808,8 +862,11 @@
       <c r="E20">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>18</v>
       </c>
@@ -821,7 +878,7 @@
       </c>
       <c r="D21" s="4"/>
     </row>
-    <row r="22" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>19</v>
       </c>
@@ -837,8 +894,11 @@
       <c r="E22">
         <v>5</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I22">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>20</v>
       </c>
@@ -854,8 +914,11 @@
       <c r="E23">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I23">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>21</v>
       </c>
@@ -871,8 +934,11 @@
       <c r="E24">
         <v>5</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I24">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="14" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>22</v>
       </c>
@@ -888,8 +954,11 @@
       <c r="E25">
         <v>5</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="I25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="13" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" sort="0" autoFilter="0" pivotTables="0"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>